<commit_message>
Adicionando a daily de 02/10 e planiha de riscos atualizada
</commit_message>
<xml_diff>
--- a/Planilha de Risco.xlsx
+++ b/Planilha de Risco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A5CE36-D512-4612-9320-F695B097D5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B38DC05-2D22-4C04-A06D-A2FF0A69E63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2868" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{4BC422F0-5053-4A48-9E5F-520D8B49CD83}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4BC422F0-5053-4A48-9E5F-520D8B49CD83}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Risco</t>
   </si>
@@ -77,12 +77,6 @@
     <t>Falha nos sensores</t>
   </si>
   <si>
-    <t>Uso de um gerador de energia reserva</t>
-  </si>
-  <si>
-    <t>Gerenciar o uso de  energia</t>
-  </si>
-  <si>
     <t>Realizar verificações diárias</t>
   </si>
   <si>
@@ -93,6 +87,36 @@
   </si>
   <si>
     <t>Interferência magnética</t>
+  </si>
+  <si>
+    <t>Usar materiais de blindagem</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Como as orquideas requerem cuidado constante, as estufas são preparadas para para qualquer evento que possa afetar as suas plantações</t>
+  </si>
+  <si>
+    <t>Uso de um gerador de energia reserva, como por exemplo o Nobreak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qualquer plantação requer o uso constante de umidade para o seu tratamento, isso junto a falta de experiência aos nossos clientes, as chances de oxidação se tornam maiores </t>
+  </si>
+  <si>
+    <t>Dificilmente ocorre algum problema nos sensores, geralmente quando acontece, é devido a um defeito de fábrica,  uma má configuração é dificil de ocorrer já que os sensores serão preparados por nós</t>
+  </si>
+  <si>
+    <t>Pelo fato dos dados gerados pelos nossos sensores serem encaminhados ao nosso banco de dados de forma remota, as chances de haver alguma interferência tende a ser maior, devido as máquinas que são utilizadas nas estufas</t>
+  </si>
+  <si>
+    <t>Uso de dispositivos de proteção contra surtos(DPS) como filtros de linha, entre outros</t>
+  </si>
+  <si>
+    <t>Devido ao fato do nosso cliente ser os agricultores, a falta de conhecimento em componentes tecnológicos pode resultar numa chance maior de impacto nos componentes do nosso produto</t>
+  </si>
+  <si>
+    <t>Por já utilizarem componentes elétricos nas estufas, o nosso cliente já possui previamente o conhecimento para evitar queimas nos componentes</t>
   </si>
 </sst>
 </file>
@@ -188,17 +212,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,137 +605,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D015AE-DC3A-44C0-A432-CE61C1D92E7D}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="47.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="3" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="7" spans="1:7" ht="108" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:C1048576">
+  <conditionalFormatting sqref="C1:D1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Alto"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Adicionando backlog, planilha de risco atualizada, daily do dia 03/10 e planejamento da sprint2C
</commit_message>
<xml_diff>
--- a/Planilha de Risco.xlsx
+++ b/Planilha de Risco.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\OrchisSystems\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B38DC05-2D22-4C04-A06D-A2FF0A69E63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3535941-F916-44D0-A4FC-95587DE69628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4BC422F0-5053-4A48-9E5F-520D8B49CD83}"/>
   </bookViews>
@@ -36,87 +36,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Risco</t>
   </si>
   <si>
-    <t>Probabilidade</t>
-  </si>
-  <si>
-    <t>Impacto</t>
-  </si>
-  <si>
-    <t>Estratégia de Mitigação</t>
-  </si>
-  <si>
-    <t>Legenda</t>
-  </si>
-  <si>
-    <t>Baixo</t>
-  </si>
-  <si>
-    <t>Médio</t>
-  </si>
-  <si>
-    <t>Alto</t>
-  </si>
-  <si>
-    <t>Queima dos componentes</t>
-  </si>
-  <si>
-    <t>Queda de energia</t>
-  </si>
-  <si>
-    <t>Impacto no produto durante o seu manuseio</t>
-  </si>
-  <si>
-    <t>Oxidação pela umidade da estufa</t>
-  </si>
-  <si>
-    <t>Falha nos sensores</t>
-  </si>
-  <si>
-    <t>Realizar verificações diárias</t>
-  </si>
-  <si>
-    <t>Uso de proteção nos componentes</t>
-  </si>
-  <si>
-    <t>Treinamento para o uso correto do produto</t>
-  </si>
-  <si>
-    <t>Interferência magnética</t>
-  </si>
-  <si>
-    <t>Usar materiais de blindagem</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Como as orquideas requerem cuidado constante, as estufas são preparadas para para qualquer evento que possa afetar as suas plantações</t>
-  </si>
-  <si>
-    <t>Uso de um gerador de energia reserva, como por exemplo o Nobreak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qualquer plantação requer o uso constante de umidade para o seu tratamento, isso junto a falta de experiência aos nossos clientes, as chances de oxidação se tornam maiores </t>
-  </si>
-  <si>
-    <t>Dificilmente ocorre algum problema nos sensores, geralmente quando acontece, é devido a um defeito de fábrica,  uma má configuração é dificil de ocorrer já que os sensores serão preparados por nós</t>
-  </si>
-  <si>
-    <t>Pelo fato dos dados gerados pelos nossos sensores serem encaminhados ao nosso banco de dados de forma remota, as chances de haver alguma interferência tende a ser maior, devido as máquinas que são utilizadas nas estufas</t>
-  </si>
-  <si>
-    <t>Uso de dispositivos de proteção contra surtos(DPS) como filtros de linha, entre outros</t>
-  </si>
-  <si>
-    <t>Devido ao fato do nosso cliente ser os agricultores, a falta de conhecimento em componentes tecnológicos pode resultar numa chance maior de impacto nos componentes do nosso produto</t>
-  </si>
-  <si>
-    <t>Por já utilizarem componentes elétricos nas estufas, o nosso cliente já possui previamente o conhecimento para evitar queimas nos componentes</t>
+    <t>Falta de conhecimento no tema</t>
+  </si>
+  <si>
+    <t>Ferramente Nova</t>
+  </si>
+  <si>
+    <t>Atrasos nas entregas</t>
+  </si>
+  <si>
+    <t>Mal planejamento</t>
+  </si>
+  <si>
+    <t>Dificuldade de comunicação entre a equipe</t>
+  </si>
+  <si>
+    <t>Saída de integrantes</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Como?</t>
+  </si>
+  <si>
+    <t>Probabilidade(P)
+ 1-Baixa
+ 2- Média
+ 3 - Alta</t>
+  </si>
+  <si>
+    <t>Impacto(I) 1 - Baixo
+ 2 - Médio 3 - Alto</t>
+  </si>
+  <si>
+    <t>Ação 
+- Eliminar
+ - Mitigar</t>
+  </si>
+  <si>
+    <t>Fator de Risco
+(P) x (I)</t>
   </si>
 </sst>
 </file>
@@ -147,30 +112,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -212,32 +159,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,161 +534,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D015AE-DC3A-44C0-A432-CE61C1D92E7D}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="8" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="108" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:D1048576">
+  <conditionalFormatting sqref="C1:E1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Alto"</formula>
     </cfRule>

</xml_diff>